<commit_message>
Back to basics: got 4 tasks running on ESP doing dumbed-down versions of udp tx, rx, and serial tx,rx
</commit_message>
<xml_diff>
--- a/Circuit/R6/R6_BOM.xlsx
+++ b/Circuit/R6/R6_BOM.xlsx
@@ -1155,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>